<commit_message>
Add ability to list multiple join rows
</commit_message>
<xml_diff>
--- a/inst/extdata/demo-template-count.xlsx
+++ b/inst/extdata/demo-template-count.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aylapearson/Code/chktemplate/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{809CACE0-79A9-9C4A-BADC-B6C6CDC203F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F865718-4C9B-9849-AF2F-58177F902434}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-29940" yWindow="2880" windowWidth="27640" windowHeight="16940" activeTab="2" xr2:uid="{A9374AC4-1834-974E-961D-F30EBF59E06D}"/>
+    <workbookView xWindow="1660" yWindow="2980" windowWidth="27640" windowHeight="16940" activeTab="2" xr2:uid="{A9374AC4-1834-974E-961D-F30EBF59E06D}"/>
   </bookViews>
   <sheets>
     <sheet name="visit" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="36">
   <si>
     <t>name</t>
   </si>
@@ -58,9 +58,6 @@
     <t>unique</t>
   </si>
   <si>
-    <t>join</t>
-  </si>
-  <si>
     <t>year</t>
   </si>
   <si>
@@ -143,6 +140,12 @@
   </si>
   <si>
     <t>c(1L, 100L)</t>
+  </si>
+  <si>
+    <t>join1</t>
+  </si>
+  <si>
+    <t>join2</t>
   </si>
 </sst>
 </file>
@@ -496,8 +499,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D74AF9AD-E1A6-B14F-A841-F85D81C1726B}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E7"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -515,16 +518,16 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>8</v>
       </c>
-      <c r="D1" t="s">
-        <v>9</v>
-      </c>
       <c r="E1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -546,16 +549,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
         <v>16</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>17</v>
       </c>
-      <c r="D3" t="s">
-        <v>18</v>
-      </c>
       <c r="E3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -563,16 +566,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
         <v>13</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>14</v>
       </c>
-      <c r="D4" t="s">
-        <v>15</v>
-      </c>
       <c r="E4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -599,7 +602,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -611,8 +614,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03F5B5D0-EFD8-BE48-B06B-28D011DF75CD}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C5"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -622,10 +625,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
         <v>10</v>
-      </c>
-      <c r="C1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -638,10 +641,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" t="s">
         <v>21</v>
-      </c>
-      <c r="C3" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -649,10 +652,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -665,7 +668,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -675,10 +678,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02E157EF-14CF-2849-9CDC-47AA99252C21}">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -692,28 +695,28 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>8</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" t="s">
         <v>9</v>
       </c>
-      <c r="E1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>10</v>
       </c>
-      <c r="G1" t="s">
-        <v>11</v>
-      </c>
       <c r="H1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" t="s">
         <v>24</v>
-      </c>
-      <c r="I1" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -730,16 +733,16 @@
         <v>23</v>
       </c>
       <c r="E2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" t="s">
         <v>30</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>31</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>32</v>
-      </c>
-      <c r="H2" t="s">
-        <v>33</v>
       </c>
       <c r="I2">
         <v>2</v>
@@ -750,28 +753,28 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
         <v>16</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>17</v>
       </c>
-      <c r="D3" t="s">
-        <v>18</v>
-      </c>
       <c r="E3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" t="s">
         <v>20</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>21</v>
       </c>
-      <c r="G3" t="s">
-        <v>22</v>
-      </c>
       <c r="H3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I3" t="s">
         <v>28</v>
-      </c>
-      <c r="I3" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -779,28 +782,28 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
         <v>13</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>14</v>
       </c>
-      <c r="D4" t="s">
-        <v>15</v>
-      </c>
       <c r="E4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -836,22 +839,27 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>34</v>
       </c>
       <c r="B7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>35</v>
+      </c>
+      <c r="F8" t="s">
         <v>26</v>
-      </c>
-      <c r="C7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" t="s">
-        <v>26</v>
-      </c>
-      <c r="E7" t="s">
-        <v>26</v>
-      </c>
-      <c r="F7" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated format fixes #11
</commit_message>
<xml_diff>
--- a/inst/extdata/demo-template-count.xlsx
+++ b/inst/extdata/demo-template-count.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aylapearson/Code/chktemplate/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F865718-4C9B-9849-AF2F-58177F902434}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C273382-B2E6-6F45-ABDC-001C2A892BDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1660" yWindow="2980" windowWidth="27640" windowHeight="16940" activeTab="2" xr2:uid="{A9374AC4-1834-974E-961D-F30EBF59E06D}"/>
+    <workbookView xWindow="-28900" yWindow="2120" windowWidth="27640" windowHeight="16940" activeTab="2" xr2:uid="{A9374AC4-1834-974E-961D-F30EBF59E06D}"/>
   </bookViews>
   <sheets>
     <sheet name="visit" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="35">
   <si>
     <t>name</t>
   </si>
@@ -131,9 +131,6 @@
   </si>
   <si>
     <t>John</t>
-  </si>
-  <si>
-    <t>Jane</t>
   </si>
   <si>
     <t>black bear</t>
@@ -602,7 +599,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -668,7 +665,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -678,19 +675,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02E157EF-14CF-2849-9CDC-47AA99252C21}">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="7" max="7" width="21" customWidth="1"/>
-    <col min="8" max="8" width="18.6640625" customWidth="1"/>
+    <col min="7" max="7" width="18.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -710,16 +706,13 @@
         <v>9</v>
       </c>
       <c r="G1" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="H1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -741,14 +734,11 @@
       <c r="G2" t="s">
         <v>31</v>
       </c>
-      <c r="H2" t="s">
-        <v>32</v>
-      </c>
-      <c r="I2">
+      <c r="H2">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -768,16 +758,13 @@
         <v>20</v>
       </c>
       <c r="G3" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="H3" t="s">
-        <v>27</v>
-      </c>
-      <c r="I3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -797,16 +784,13 @@
         <v>18</v>
       </c>
       <c r="G4" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="H4" t="s">
-        <v>18</v>
-      </c>
-      <c r="I4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -825,21 +809,18 @@
       <c r="F5" t="b">
         <v>1</v>
       </c>
-      <c r="H5" t="b">
-        <v>1</v>
-      </c>
-      <c r="I5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B7" t="s">
         <v>25</v>
@@ -854,9 +835,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F8" t="s">
         <v>26</v>

</xml_diff>